<commit_message>
UPDATE: Genetik und Überarbeitung
</commit_message>
<xml_diff>
--- a/neue Bilder/Magie.xlsx
+++ b/neue Bilder/Magie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\MagicMittelalterStory\neue Bilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BC404B-A81E-4286-B526-B145A249ECCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBFFBE1-B9EE-433C-91F1-3133F0F305CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40198EB0-CCB8-4903-9D95-70B548E0B832}"/>
+    <workbookView xWindow="28680" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{40198EB0-CCB8-4903-9D95-70B548E0B832}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
   <si>
     <t>Licht</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>entstanden durch intermediäre Vermischung von Wechselstrom und Licht</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -580,70 +583,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -960,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C80A18B-079A-4884-A8A8-354644E41D05}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +982,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
+      <c r="A1" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1009,7 +1014,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1041,7 +1046,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1059,7 @@
       <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="18" t="s">
         <v>116</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -1071,7 +1076,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1103,7 +1108,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1138,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="37" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1165,7 +1170,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1195,7 +1200,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="37" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1227,7 +1232,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="10" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1262,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1289,8 +1294,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="18" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1319,7 +1324,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="37" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1351,7 +1356,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="10" t="s">
         <v>0</v>
       </c>
@@ -1376,12 +1381,12 @@
       <c r="I13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1413,7 +1418,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="10" t="s">
         <v>9</v>
       </c>
@@ -1443,7 +1448,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="37" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1475,7 +1480,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="10" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1510,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="38" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1537,7 +1542,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="10" t="s">
         <v>10</v>
       </c>
@@ -1553,7 +1558,7 @@
       <c r="F19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="10" t="s">
@@ -1571,10 +1576,10 @@
       <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1589,10 +1594,10 @@
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="25"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="4" t="s">
         <v>28</v>
       </c>
@@ -1610,17 +1615,17 @@
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="27"/>
+      <c r="C24" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="21"/>
       <c r="E24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="22" t="s">
+      <c r="F24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1631,17 +1636,17 @@
       <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="27"/>
+      <c r="C25" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="21"/>
       <c r="E25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="22" t="s">
+      <c r="F25" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1652,17 +1657,17 @@
       <c r="B26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="29"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="22" t="s">
+      <c r="F26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1673,11 +1678,11 @@
       <c r="B27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="38" t="s">
+      <c r="D27" s="27"/>
+      <c r="E27" s="19" t="s">
         <v>28</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -1691,14 +1696,14 @@
       <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="33"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G28" t="s">
@@ -1712,10 +1717,10 @@
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="35"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="4" t="s">
         <v>28</v>
       </c>
@@ -1733,10 +1738,10 @@
       <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="35"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="4" t="s">
         <v>28</v>
       </c>
@@ -1751,11 +1756,11 @@
       <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="38" t="s">
+      <c r="D31" s="27"/>
+      <c r="E31" s="19" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1772,14 +1777,14 @@
       <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="37"/>
+      <c r="C32" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="29"/>
       <c r="E32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1790,30 +1795,19 @@
       <c r="B33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="27"/>
+      <c r="C33" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="21"/>
       <c r="E33" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="16" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
@@ -1824,6 +1818,17 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>